<commit_message>
- added pdf output
</commit_message>
<xml_diff>
--- a/GeneralEmbeddedCLibraries_Overview.xlsx
+++ b/GeneralEmbeddedCLibraries_Overview.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal\C_embedded\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal\C_embedded\GeneralEmbeddedCLibrary\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13635"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13635" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Revision" sheetId="1" r:id="rId1"/>
@@ -788,24 +788,6 @@
   <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -920,33 +902,30 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFC9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFDA65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBAE18F"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
@@ -1254,7 +1233,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -1270,177 +1249,177 @@
   <sheetData>
     <row r="1" spans="2:5" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="5"/>
+      <c r="D2" s="53"/>
       <c r="E2"/>
     </row>
     <row r="3" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="52" t="s">
+      <c r="B3" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="6"/>
+      <c r="D3" s="51"/>
       <c r="E3"/>
     </row>
     <row r="4" spans="2:5" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="53" t="s">
+      <c r="B4" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="48" t="s">
         <v>95</v>
       </c>
-      <c r="D4" s="7"/>
+      <c r="D4" s="49"/>
       <c r="E4"/>
     </row>
     <row r="5" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="48" t="s">
+      <c r="B6" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="49" t="s">
+      <c r="C6" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="49" t="s">
+      <c r="D6" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="50" t="s">
+      <c r="E6" s="44" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="10"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="15"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="9"/>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="10"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="15"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="9"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="10"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="15"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="9"/>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="10"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="15"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="9"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="10"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="15"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="9"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="10"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="15"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="9"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="10"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="15"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="9"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="10"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="15"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="9"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="10"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="15"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="9"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="10"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="15"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="9"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="10"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="15"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="9"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="10"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="15"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="9"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="10"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="15"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="9"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="10"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="15"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="9"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="10"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="15"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="9"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="10"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="15"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="9"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="10"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="15"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="9"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="10"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="15"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="9"/>
     </row>
     <row r="26" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="12"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="16"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1457,8 +1436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M29"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScale="40" zoomScaleNormal="55" zoomScalePageLayoutView="40" workbookViewId="0">
+      <selection activeCell="T14" sqref="T14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1471,7 +1450,8 @@
     <col min="6" max="6" width="19.42578125" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
     <col min="8" max="8" width="35.28515625" customWidth="1"/>
-    <col min="9" max="10" width="14.28515625" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="26.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="60.7109375" customWidth="1"/>
     <col min="13" max="13" width="62.28515625" customWidth="1"/>
@@ -1479,831 +1459,831 @@
   <sheetData>
     <row r="1" spans="2:13" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:13" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="44" t="s">
+      <c r="D2" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="E2" s="45" t="s">
+      <c r="E2" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="45" t="s">
+      <c r="F2" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="46" t="s">
+      <c r="G2" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="46" t="s">
+      <c r="H2" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="45" t="s">
+      <c r="I2" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="J2" s="46" t="s">
+      <c r="J2" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="45" t="s">
+      <c r="K2" s="39" t="s">
         <v>96</v>
       </c>
-      <c r="L2" s="46" t="s">
+      <c r="L2" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="M2" s="47" t="s">
+      <c r="M2" s="41" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B3" s="39">
+      <c r="B3" s="33">
         <v>1</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="33" t="s">
+      <c r="D3" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="E3" s="32" t="s">
+      <c r="E3" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="32" t="s">
+      <c r="F3" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="32" t="s">
+      <c r="G3" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="H3" s="33" t="s">
+      <c r="H3" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="I3" s="41">
+      <c r="I3" s="35">
         <v>2</v>
       </c>
-      <c r="J3" s="32" t="s">
+      <c r="J3" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="33" t="s">
+      <c r="K3" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="L3" s="35" t="s">
+      <c r="L3" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="M3" s="37" t="s">
+      <c r="M3" s="31" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="4" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B4" s="40">
+      <c r="B4" s="34">
         <v>2</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="26" t="s">
+      <c r="D4" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="E4" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="F4" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="21" t="s">
+      <c r="G4" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="24" t="s">
+      <c r="H4" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="I4" s="42">
+      <c r="I4" s="36">
         <v>0</v>
       </c>
-      <c r="J4" s="21" t="s">
+      <c r="J4" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="K4" s="26" t="s">
+      <c r="K4" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="L4" s="25" t="s">
+      <c r="L4" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="M4" s="28"/>
+      <c r="M4" s="22"/>
     </row>
     <row r="5" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="40">
+      <c r="B5" s="34">
         <v>3</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="D5" s="26" t="s">
+      <c r="D5" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="E5" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="21" t="s">
+      <c r="F5" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="30"/>
-      <c r="H5" s="30"/>
-      <c r="I5" s="42">
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="36">
         <v>2</v>
       </c>
-      <c r="J5" s="21" t="s">
+      <c r="J5" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="K5" s="26" t="s">
+      <c r="K5" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="L5" s="25" t="s">
+      <c r="L5" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="M5" s="31" t="s">
+      <c r="M5" s="25" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="6" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="40">
+      <c r="B6" s="34">
         <v>4</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="D6" s="26" t="s">
+      <c r="D6" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="E6" s="21" t="s">
+      <c r="E6" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="21" t="s">
+      <c r="F6" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="21" t="s">
+      <c r="G6" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="H6" s="26" t="s">
+      <c r="H6" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="I6" s="42">
+      <c r="I6" s="36">
         <v>1</v>
       </c>
-      <c r="J6" s="21" t="s">
+      <c r="J6" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="K6" s="26" t="s">
+      <c r="K6" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="L6" s="25" t="s">
+      <c r="L6" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="M6" s="29" t="s">
+      <c r="M6" s="23" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="7" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B7" s="40">
+      <c r="B7" s="34">
         <v>5</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="D7" s="26" t="s">
+      <c r="D7" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="E7" s="21" t="s">
+      <c r="E7" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="21" t="s">
+      <c r="F7" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="30"/>
-      <c r="H7" s="30"/>
-      <c r="I7" s="42">
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="36">
         <v>0</v>
       </c>
-      <c r="J7" s="21" t="s">
+      <c r="J7" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="K7" s="26" t="s">
+      <c r="K7" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="L7" s="25" t="s">
+      <c r="L7" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="M7" s="31" t="s">
+      <c r="M7" s="25" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="8" spans="2:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="B8" s="40">
+      <c r="B8" s="34">
         <v>6</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="D8" s="26" t="s">
+      <c r="D8" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="E8" s="21" t="s">
+      <c r="E8" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="21" t="s">
+      <c r="F8" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="21" t="s">
+      <c r="G8" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="H8" s="26" t="s">
+      <c r="H8" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="I8" s="42">
+      <c r="I8" s="36">
         <v>3</v>
       </c>
-      <c r="J8" s="21" t="s">
+      <c r="J8" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="K8" s="26" t="s">
+      <c r="K8" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="L8" s="25" t="s">
+      <c r="L8" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="M8" s="29" t="s">
+      <c r="M8" s="23" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="9" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B9" s="40">
+      <c r="B9" s="34">
         <v>7</v>
       </c>
-      <c r="C9" s="21" t="s">
+      <c r="C9" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="D9" s="26" t="s">
+      <c r="D9" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="E9" s="21" t="s">
+      <c r="E9" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="21" t="s">
+      <c r="F9" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="21" t="s">
+      <c r="G9" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="H9" s="21" t="s">
+      <c r="H9" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="I9" s="42">
+      <c r="I9" s="36">
         <v>0</v>
       </c>
-      <c r="J9" s="21" t="s">
+      <c r="J9" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="K9" s="26" t="s">
+      <c r="K9" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="L9" s="25" t="s">
+      <c r="L9" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="M9" s="19"/>
+      <c r="M9" s="13"/>
     </row>
     <row r="10" spans="2:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="B10" s="40">
+      <c r="B10" s="34">
         <v>8</v>
       </c>
-      <c r="C10" s="21" t="s">
+      <c r="C10" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="26" t="s">
+      <c r="D10" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="E10" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="F10" s="21" t="s">
+      <c r="F10" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="G10" s="21" t="s">
+      <c r="G10" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="H10" s="26" t="s">
+      <c r="H10" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="I10" s="42">
+      <c r="I10" s="36">
         <v>0</v>
       </c>
-      <c r="J10" s="21" t="s">
+      <c r="J10" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="K10" s="26" t="s">
+      <c r="K10" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="L10" s="25" t="s">
+      <c r="L10" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="M10" s="28"/>
+      <c r="M10" s="22"/>
     </row>
     <row r="11" spans="2:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="B11" s="40">
+      <c r="B11" s="34">
         <v>9</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="C11" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="D11" s="26" t="s">
+      <c r="D11" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="E11" s="21" t="s">
+      <c r="E11" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="21" t="s">
+      <c r="F11" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="G11" s="21" t="s">
+      <c r="G11" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="H11" s="26" t="s">
+      <c r="H11" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="I11" s="42">
+      <c r="I11" s="36">
         <v>2</v>
       </c>
-      <c r="J11" s="21" t="s">
+      <c r="J11" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="K11" s="26" t="s">
+      <c r="K11" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="L11" s="25" t="s">
+      <c r="L11" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="M11" s="29" t="s">
+      <c r="M11" s="23" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="12" spans="2:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="B12" s="40">
+      <c r="B12" s="34">
         <v>10</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="C12" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="26" t="s">
+      <c r="D12" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="E12" s="21" t="s">
+      <c r="E12" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="F12" s="21" t="s">
+      <c r="F12" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="G12" s="21" t="s">
+      <c r="G12" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="H12" s="26" t="s">
+      <c r="H12" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="I12" s="42">
+      <c r="I12" s="36">
         <v>5</v>
       </c>
-      <c r="J12" s="21" t="s">
+      <c r="J12" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="K12" s="26" t="s">
+      <c r="K12" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="L12" s="25" t="s">
+      <c r="L12" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="M12" s="29" t="s">
+      <c r="M12" s="23" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="13" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B13" s="40">
+      <c r="B13" s="34">
         <v>11</v>
       </c>
-      <c r="C13" s="21" t="s">
+      <c r="C13" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="D13" s="26" t="s">
+      <c r="D13" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="E13" s="21" t="s">
+      <c r="E13" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="21" t="s">
+      <c r="F13" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="G13" s="30" t="s">
+      <c r="G13" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="H13" s="30"/>
-      <c r="I13" s="42">
+      <c r="H13" s="24"/>
+      <c r="I13" s="36">
         <v>3</v>
       </c>
-      <c r="J13" s="21" t="s">
+      <c r="J13" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="K13" s="26" t="s">
+      <c r="K13" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="L13" s="25" t="s">
+      <c r="L13" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="M13" s="29" t="s">
+      <c r="M13" s="23" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="14" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B14" s="40">
+      <c r="B14" s="34">
         <v>12</v>
       </c>
-      <c r="C14" s="21" t="s">
+      <c r="C14" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="D14" s="26" t="s">
+      <c r="D14" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="E14" s="21" t="s">
+      <c r="E14" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="F14" s="21" t="s">
+      <c r="F14" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="G14" s="21" t="s">
+      <c r="G14" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="H14" s="21" t="s">
+      <c r="H14" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="I14" s="42">
+      <c r="I14" s="36">
         <v>0</v>
       </c>
-      <c r="J14" s="21" t="s">
+      <c r="J14" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="K14" s="26" t="s">
+      <c r="K14" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="L14" s="25" t="s">
+      <c r="L14" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="M14" s="19"/>
+      <c r="M14" s="13"/>
     </row>
     <row r="15" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B15" s="40">
+      <c r="B15" s="34">
         <v>13</v>
       </c>
-      <c r="C15" s="21" t="s">
+      <c r="C15" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="D15" s="26" t="s">
+      <c r="D15" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="E15" s="21" t="s">
+      <c r="E15" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="F15" s="21" t="s">
+      <c r="F15" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="G15" s="21" t="s">
+      <c r="G15" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="H15" s="21" t="s">
+      <c r="H15" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="I15" s="42">
+      <c r="I15" s="36">
         <v>0</v>
       </c>
-      <c r="J15" s="21" t="s">
+      <c r="J15" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="K15" s="26" t="s">
+      <c r="K15" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="L15" s="25" t="s">
+      <c r="L15" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="M15" s="19"/>
+      <c r="M15" s="13"/>
     </row>
     <row r="16" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B16" s="40">
+      <c r="B16" s="34">
         <v>14</v>
       </c>
-      <c r="C16" s="21" t="s">
+      <c r="C16" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="D16" s="26" t="s">
+      <c r="D16" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="E16" s="21" t="s">
+      <c r="E16" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F16" s="21" t="s">
+      <c r="F16" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="G16" s="30" t="s">
+      <c r="G16" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="H16" s="30"/>
-      <c r="I16" s="42">
+      <c r="H16" s="24"/>
+      <c r="I16" s="36">
         <v>0</v>
       </c>
-      <c r="J16" s="21" t="s">
+      <c r="J16" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="K16" s="26" t="s">
+      <c r="K16" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="L16" s="25" t="s">
+      <c r="L16" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="M16" s="31" t="s">
+      <c r="M16" s="25" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="17" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B17" s="40">
+      <c r="B17" s="34">
         <v>15</v>
       </c>
-      <c r="C17" s="21" t="s">
+      <c r="C17" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="D17" s="26" t="s">
+      <c r="D17" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="E17" s="21" t="s">
+      <c r="E17" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F17" s="21" t="s">
+      <c r="F17" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="G17" s="21" t="s">
+      <c r="G17" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="H17" s="26" t="s">
+      <c r="H17" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="I17" s="42">
+      <c r="I17" s="36">
         <v>0</v>
       </c>
-      <c r="J17" s="21" t="s">
+      <c r="J17" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="K17" s="26" t="s">
+      <c r="K17" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="L17" s="25" t="s">
+      <c r="L17" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="M17" s="19"/>
+      <c r="M17" s="13"/>
     </row>
     <row r="18" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B18" s="40">
+      <c r="B18" s="34">
         <v>16</v>
       </c>
-      <c r="C18" s="24" t="s">
+      <c r="C18" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="34" t="s">
+      <c r="D18" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="E18" s="24" t="s">
+      <c r="E18" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="F18" s="24" t="s">
+      <c r="F18" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="G18" s="24" t="s">
+      <c r="G18" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="H18" s="22" t="s">
+      <c r="H18" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="I18" s="22">
+      <c r="I18" s="16">
         <v>0</v>
       </c>
-      <c r="J18" s="24" t="s">
+      <c r="J18" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="K18" s="26" t="s">
+      <c r="K18" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="L18" s="36" t="s">
+      <c r="L18" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="M18" s="38" t="s">
+      <c r="M18" s="32" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="19" spans="2:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="B19" s="40">
+      <c r="B19" s="34">
         <v>17</v>
       </c>
-      <c r="C19" s="21" t="s">
+      <c r="C19" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="D19" s="26" t="s">
+      <c r="D19" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="E19" s="21" t="s">
+      <c r="E19" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F19" s="21" t="s">
+      <c r="F19" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="G19" s="21" t="s">
+      <c r="G19" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="H19" s="27" t="s">
+      <c r="H19" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="I19" s="42">
+      <c r="I19" s="36">
         <v>1</v>
       </c>
-      <c r="J19" s="21" t="s">
+      <c r="J19" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="K19" s="26" t="s">
+      <c r="K19" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="L19" s="25" t="s">
+      <c r="L19" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="M19" s="29" t="s">
+      <c r="M19" s="23" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="20" spans="2:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="40">
+      <c r="B20" s="34">
         <v>18</v>
       </c>
-      <c r="C20" s="21"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="22"/>
-      <c r="J20" s="21"/>
-      <c r="K20" s="21"/>
-      <c r="L20" s="21"/>
-      <c r="M20" s="19"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="15"/>
+      <c r="M20" s="13"/>
     </row>
     <row r="21" spans="2:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="40">
+      <c r="B21" s="34">
         <v>19</v>
       </c>
-      <c r="C21" s="21"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="21"/>
-      <c r="I21" s="22"/>
-      <c r="J21" s="21"/>
-      <c r="K21" s="21"/>
-      <c r="L21" s="21"/>
-      <c r="M21" s="19"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="15"/>
+      <c r="L21" s="15"/>
+      <c r="M21" s="13"/>
     </row>
     <row r="22" spans="2:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="40">
+      <c r="B22" s="34">
         <v>20</v>
       </c>
-      <c r="C22" s="21"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="21"/>
-      <c r="H22" s="21"/>
-      <c r="I22" s="22"/>
-      <c r="J22" s="21"/>
-      <c r="K22" s="21"/>
-      <c r="L22" s="21"/>
-      <c r="M22" s="19"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="16"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="15"/>
+      <c r="L22" s="15"/>
+      <c r="M22" s="13"/>
     </row>
     <row r="23" spans="2:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="40">
+      <c r="B23" s="34">
         <v>21</v>
       </c>
-      <c r="C23" s="21"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="21"/>
-      <c r="H23" s="21"/>
-      <c r="I23" s="22"/>
-      <c r="J23" s="21"/>
-      <c r="K23" s="21"/>
-      <c r="L23" s="21"/>
-      <c r="M23" s="19"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="15"/>
+      <c r="L23" s="15"/>
+      <c r="M23" s="13"/>
     </row>
     <row r="24" spans="2:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="40">
+      <c r="B24" s="34">
         <v>22</v>
       </c>
-      <c r="C24" s="21"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="21"/>
-      <c r="G24" s="21"/>
-      <c r="H24" s="21"/>
-      <c r="I24" s="22"/>
-      <c r="J24" s="21"/>
-      <c r="K24" s="21"/>
-      <c r="L24" s="21"/>
-      <c r="M24" s="19"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="16"/>
+      <c r="J24" s="15"/>
+      <c r="K24" s="15"/>
+      <c r="L24" s="15"/>
+      <c r="M24" s="13"/>
     </row>
     <row r="25" spans="2:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="40">
+      <c r="B25" s="34">
         <v>23</v>
       </c>
-      <c r="C25" s="21"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="21"/>
-      <c r="I25" s="21"/>
-      <c r="J25" s="21"/>
-      <c r="K25" s="21"/>
-      <c r="L25" s="21"/>
-      <c r="M25" s="19"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="15"/>
+      <c r="I25" s="15"/>
+      <c r="J25" s="15"/>
+      <c r="K25" s="15"/>
+      <c r="L25" s="15"/>
+      <c r="M25" s="13"/>
     </row>
     <row r="26" spans="2:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="40">
+      <c r="B26" s="34">
         <v>24</v>
       </c>
-      <c r="C26" s="21"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="21"/>
-      <c r="I26" s="21"/>
-      <c r="J26" s="21"/>
-      <c r="K26" s="21"/>
-      <c r="L26" s="21"/>
-      <c r="M26" s="19"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="15"/>
+      <c r="I26" s="15"/>
+      <c r="J26" s="15"/>
+      <c r="K26" s="15"/>
+      <c r="L26" s="15"/>
+      <c r="M26" s="13"/>
     </row>
     <row r="27" spans="2:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="40">
+      <c r="B27" s="34">
         <v>25</v>
       </c>
-      <c r="C27" s="23"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="23"/>
-      <c r="G27" s="23"/>
-      <c r="H27" s="23"/>
-      <c r="I27" s="23"/>
-      <c r="J27" s="23"/>
-      <c r="K27" s="23"/>
-      <c r="L27" s="23"/>
-      <c r="M27" s="20"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="17"/>
+      <c r="J27" s="17"/>
+      <c r="K27" s="17"/>
+      <c r="L27" s="17"/>
+      <c r="M27" s="14"/>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B28" s="17"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
-      <c r="H28" s="18"/>
-      <c r="I28" s="18"/>
-      <c r="J28" s="18"/>
-      <c r="K28" s="18"/>
-      <c r="L28" s="18"/>
-      <c r="M28" s="18"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="12"/>
+      <c r="L28" s="12"/>
+      <c r="M28" s="12"/>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B29" s="17"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
-      <c r="H29" s="18"/>
-      <c r="I29" s="18"/>
-      <c r="J29" s="18"/>
-      <c r="K29" s="18"/>
-      <c r="L29" s="18"/>
-      <c r="M29" s="18"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="12"/>
+      <c r="K29" s="12"/>
+      <c r="L29" s="12"/>
+      <c r="M29" s="12"/>
     </row>
   </sheetData>
   <autoFilter ref="C2:M27"/>
   <conditionalFormatting sqref="F3:F27">
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="RELEASED">
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="RELEASED">
       <formula>NOT(ISERROR(SEARCH("RELEASED",F3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="IN DEVELOPMENT">
+    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="IN DEVELOPMENT">
       <formula>NOT(ISERROR(SEARCH("IN DEVELOPMENT",F3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="ON HOLD">
+    <cfRule type="containsText" dxfId="0" priority="6" operator="containsText" text="ON HOLD">
       <formula>NOT(ISERROR(SEARCH("ON HOLD",F3)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2332,5 +2312,6 @@
     <hyperlink ref="L5" r:id="rId17"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="26" orientation="landscape" r:id="rId18"/>
 </worksheet>
 </file>
</xml_diff>